<commit_message>
update of 28th august
</commit_message>
<xml_diff>
--- a/src/assets/Excel/Demo_Block_Detailstemplate_New.xlsx
+++ b/src/assets/Excel/Demo_Block_Detailstemplate_New.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\oyespace6-5-2020\18-05-2020\OyeSocietyWeb\src\assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC009F7-3C63-4C0E-96B7-9BFABAEAA56F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D101753-3478-4A1A-B9C3-ABF5CC65EEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Sno</t>
   </si>
@@ -28,15 +28,9 @@
     <t>blockname</t>
   </si>
   <si>
-    <t>blocktype</t>
-  </si>
-  <si>
     <t>units</t>
   </si>
   <si>
-    <t>managername</t>
-  </si>
-  <si>
     <t>managermobileno</t>
   </si>
   <si>
@@ -44,9 +38,6 @@
   </si>
   <si>
     <t>JSWB100</t>
-  </si>
-  <si>
-    <t>Residential</t>
   </si>
   <si>
     <t>SAM</t>
@@ -66,9 +57,6 @@
     <t>JSWB101</t>
   </si>
   <si>
-    <t>Commercial</t>
-  </si>
-  <si>
     <t>JPHN</t>
   </si>
   <si>
@@ -86,9 +74,6 @@
     <t>JSWB102</t>
   </si>
   <si>
-    <t>Residential and Commercial</t>
-  </si>
-  <si>
     <t>SATYA</t>
   </si>
   <si>
@@ -108,6 +93,9 @@
   </si>
   <si>
     <t>DADY</t>
+  </si>
+  <si>
+    <t>fecilitymanagername</t>
   </si>
 </sst>
 </file>
@@ -1478,25 +1466,24 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IU10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
+    <col min="7" max="255" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.25" customHeight="1">
+    <row r="1" spans="1:6" ht="32.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1507,196 +1494,167 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>8197399604</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4">
-        <v>8197399604</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" customHeight="1">
+    <row r="3" spans="1:6" ht="14.7" customHeight="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
         <v>8197399604</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.15" customHeight="1">
+    <row r="4" spans="1:6" ht="15.15" customHeight="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4">
         <v>8197399604</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.15" customHeight="1">
+    <row r="5" spans="1:6" ht="15.15" customHeight="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
         <v>8197399604</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.15" customHeight="1">
+    <row r="6" spans="1:6" ht="15.15" customHeight="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4">
         <v>8197399604</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.15" customHeight="1">
+    <row r="7" spans="1:6" ht="15.15" customHeight="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4">
         <v>8197399604</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>14</v>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.7" customHeight="1">
+    <row r="8" spans="1:6" ht="14.7" customHeight="1">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="14.7" customHeight="1">
+    <row r="9" spans="1:6" ht="14.7" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="14.7" customHeight="1">
+    <row r="10" spans="1:6" ht="14.7" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{14D60CE0-C804-42C5-9470-32C762C64AA8}">
-      <formula1>"Residential,Commercial,Residential and Commercial"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
update of 2nd september
</commit_message>
<xml_diff>
--- a/src/assets/Excel/Demo_Block_Detailstemplate_New.xlsx
+++ b/src/assets/Excel/Demo_Block_Detailstemplate_New.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anusha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\oyespace6-5-2020\18-05-2020\OyeSocietyWeb\src\assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D101753-3478-4A1A-B9C3-ABF5CC65EEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423540A2-503D-4584-A6F8-6740E14E4D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,6 @@
     <t>units</t>
   </si>
   <si>
-    <t>managermobileno</t>
-  </si>
-  <si>
-    <t>manageremailid</t>
-  </si>
-  <si>
     <t>JSWB100</t>
   </si>
   <si>
@@ -95,7 +89,13 @@
     <t>DADY</t>
   </si>
   <si>
-    <t>fecilitymanagername</t>
+    <t>facility manager</t>
+  </si>
+  <si>
+    <t>mobile number</t>
+  </si>
+  <si>
+    <t>email id</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:IU10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="15.15" customHeight="1"/>
@@ -1494,13 +1494,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
@@ -1508,19 +1508,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4">
         <v>8197399604</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.7" customHeight="1">
@@ -1528,19 +1528,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
         <v>8197399604</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.15" customHeight="1">
@@ -1548,19 +1548,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4">
         <v>8197399604</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.15" customHeight="1">
@@ -1568,19 +1568,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4">
         <v>8197399604</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.15" customHeight="1">
@@ -1588,19 +1588,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4">
         <v>8197399604</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.15" customHeight="1">
@@ -1608,19 +1608,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="4">
         <v>8197399604</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.7" customHeight="1">

</xml_diff>